<commit_message>
Ugne faile lapai DMY scores quality
</commit_message>
<xml_diff>
--- a/00_raw_data/Ugnė_nuo 2009.xlsx
+++ b/00_raw_data/Ugnė_nuo 2009.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lsdi-my.sharepoint.com/personal/vilma_kemesyte_lammc_lt/Documents/Darbalaukis/duomenys nuo 2011 m/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lsdi-my.sharepoint.com/personal/grazina_statkeviciute_lammc_lt/Documents/EditGrass4Food/MDPI_2023liepa/00_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1160" documentId="8_{5ABC9140-278D-4CF2-933E-F57CEF1061D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1352BA0F-3B10-49BC-BCE6-58C017641597}"/>
+  <xr:revisionPtr revIDLastSave="1201" documentId="8_{5ABC9140-278D-4CF2-933E-F57CEF1061D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C4BAF9E-E5C1-43F4-9E2E-139365C5D252}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4854C67A-D0E2-4A44-A6DD-6A89EBFB177C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{4854C67A-D0E2-4A44-A6DD-6A89EBFB177C}"/>
   </bookViews>
   <sheets>
     <sheet name="pirminiai" sheetId="1" r:id="rId1"/>
     <sheet name="DMY ir kt" sheetId="2" r:id="rId2"/>
     <sheet name="kokybė" sheetId="3" r:id="rId3"/>
+    <sheet name="DMY" sheetId="4" r:id="rId4"/>
+    <sheet name="scores" sheetId="5" r:id="rId5"/>
+    <sheet name="quality" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t xml:space="preserve">Žiemojimas </t>
   </si>
@@ -116,6 +119,42 @@
   </si>
   <si>
     <t>pirmi naudojimo metai</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>cut1</t>
+  </si>
+  <si>
+    <t>cut2</t>
+  </si>
+  <si>
+    <t>cut3</t>
+  </si>
+  <si>
+    <t>cut4</t>
+  </si>
+  <si>
+    <t>use_year</t>
+  </si>
+  <si>
+    <t>spring_g</t>
+  </si>
+  <si>
+    <t>wr_perc</t>
+  </si>
+  <si>
+    <t>wr_score</t>
+  </si>
+  <si>
+    <t>summer_g</t>
+  </si>
+  <si>
+    <t>spot</t>
+  </si>
+  <si>
+    <t>rust</t>
   </si>
 </sst>
 </file>
@@ -236,10 +275,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
     <cellStyle name="Įprastas 2" xfId="2" xr:uid="{DAD253B0-58B6-48FB-AFDF-6429A35964A6}"/>
     <cellStyle name="Įprastas 3" xfId="3" xr:uid="{8DCFF34A-5995-4748-B18A-672BEDA9A06F}"/>
     <cellStyle name="Įprastas 4" xfId="1" xr:uid="{E7F5F746-9DB2-425D-BEDB-A156C36CB903}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -255,7 +294,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="„Office“ tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5615,8 +5654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D376DE-4E90-4AA6-AA62-17E318B27278}">
   <dimension ref="A1:Q82"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9245,8 +9284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DF1A06-B09C-41FD-881E-94BBDD517B5B}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9454,4 +9493,3757 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0ACB72-E4C5-423F-88DE-6B7299074D25}">
+  <dimension ref="A1:F81"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>2009</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1310.5802047781572</v>
+      </c>
+      <c r="D2">
+        <v>3305.1194539249154</v>
+      </c>
+      <c r="E2">
+        <v>1706.4846416382254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2009</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2758.8168373151316</v>
+      </c>
+      <c r="D3">
+        <v>3428.3276450511948</v>
+      </c>
+      <c r="E3">
+        <v>1385.6655290102392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>2009</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2445.9613196814571</v>
+      </c>
+      <c r="D4">
+        <v>3458.475540386803</v>
+      </c>
+      <c r="E4">
+        <v>2030.7167235494883</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>2009</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1627.8388278388279</v>
+      </c>
+      <c r="D5">
+        <v>1544.3223443223444</v>
+      </c>
+      <c r="E5">
+        <v>647.61904761904759</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>2009</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>999.99999999999989</v>
+      </c>
+      <c r="D6">
+        <v>1172.1611721611723</v>
+      </c>
+      <c r="E6">
+        <v>478.24175824175825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>2009</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1267.5457875457873</v>
+      </c>
+      <c r="D7">
+        <v>2323.0769230769229</v>
+      </c>
+      <c r="E7">
+        <v>653.2967032967033</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>2010</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3455.5555555555557</v>
+      </c>
+      <c r="D8">
+        <v>2380.9777777777772</v>
+      </c>
+      <c r="E8">
+        <v>483.51111111111106</v>
+      </c>
+      <c r="F8">
+        <v>1527.7777777777776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>2010</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3683</v>
+      </c>
+      <c r="D9">
+        <v>2653.2</v>
+      </c>
+      <c r="E9">
+        <v>473.20000000000005</v>
+      </c>
+      <c r="F9">
+        <v>525.46666666666658</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>2010</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>3895.666666666667</v>
+      </c>
+      <c r="D10">
+        <v>1559.2888888888888</v>
+      </c>
+      <c r="E10">
+        <v>505</v>
+      </c>
+      <c r="F10">
+        <v>1357.9222222222222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>784.18657565415253</v>
+      </c>
+      <c r="D11">
+        <v>1295.5403868031856</v>
+      </c>
+      <c r="E11">
+        <v>2011.3765642775884</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>816.38225255972702</v>
+      </c>
+      <c r="D12">
+        <v>1321.1376564277591</v>
+      </c>
+      <c r="E12">
+        <v>1634.4027303754272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>2010</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>954.83503981797514</v>
+      </c>
+      <c r="D13">
+        <v>1680.3185437997724</v>
+      </c>
+      <c r="E13">
+        <v>1656.0182025028446</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>2011</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2980.6999485331958</v>
+      </c>
+      <c r="D14">
+        <v>3143.2712300566136</v>
+      </c>
+      <c r="E14">
+        <v>2209.4698919197117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2111.4565105506945</v>
+      </c>
+      <c r="D15">
+        <v>3843.7982501286674</v>
+      </c>
+      <c r="E15">
+        <v>2412.7225939269174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>2011</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2289.4235717961919</v>
+      </c>
+      <c r="D16">
+        <v>3452.5126093669587</v>
+      </c>
+      <c r="E16">
+        <v>2853.313432835821</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>2011</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>1117.5999999999999</v>
+      </c>
+      <c r="D17">
+        <v>1172.3799999999999</v>
+      </c>
+      <c r="E17">
+        <v>2344.4444444444443</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>2011</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>1161.4777777777779</v>
+      </c>
+      <c r="D18">
+        <v>1506.2755555555557</v>
+      </c>
+      <c r="E18">
+        <v>2172.4444444444443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>2011</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>983.18222222222221</v>
+      </c>
+      <c r="D19">
+        <v>1423.2466666666664</v>
+      </c>
+      <c r="E19">
+        <v>1827.7777777777778</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>2012</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2795.4194544518787</v>
+      </c>
+      <c r="D20">
+        <v>3773.4637159032427</v>
+      </c>
+      <c r="E20">
+        <v>2171.8991250643335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>2012</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>3788.3376222336592</v>
+      </c>
+      <c r="D21">
+        <v>2950.2830674215129</v>
+      </c>
+      <c r="E21">
+        <v>2012.5579001544006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>2012</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>4009.984559958827</v>
+      </c>
+      <c r="D22">
+        <v>2535.6664951106536</v>
+      </c>
+      <c r="E22">
+        <v>1693.2578486875966</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>2012</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>1582.0895522388059</v>
+      </c>
+      <c r="D23">
+        <v>1200.6176016469376</v>
+      </c>
+      <c r="E23">
+        <v>735.97529593412241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1220.3396809058161</v>
+      </c>
+      <c r="D24">
+        <v>848.43026248070009</v>
+      </c>
+      <c r="E24">
+        <v>436.43849716932573</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>1879.1559444158518</v>
+      </c>
+      <c r="D25">
+        <v>1224.9099330931547</v>
+      </c>
+      <c r="E25">
+        <v>1235.2032938754503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1903.370786516854</v>
+      </c>
+      <c r="D26">
+        <v>2266.4269662921342</v>
+      </c>
+      <c r="E26">
+        <v>1521.0486891385767</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>2013</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1604.4943820224719</v>
+      </c>
+      <c r="D27">
+        <v>3151.9400749063675</v>
+      </c>
+      <c r="E27">
+        <v>1141.692883895131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>2013</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1378.5842696629213</v>
+      </c>
+      <c r="D28">
+        <v>2098.3146067415732</v>
+      </c>
+      <c r="E28">
+        <v>1692.2059925093633</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>2013</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>39.958826556870818</v>
+      </c>
+      <c r="D29">
+        <v>1025.0540401441071</v>
+      </c>
+      <c r="E29">
+        <v>906.61863098301592</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>2013</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>46.752444673185799</v>
+      </c>
+      <c r="D30">
+        <v>1031.8064848172928</v>
+      </c>
+      <c r="E30">
+        <v>667.19505918682455</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>2013</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>60.524961399897066</v>
+      </c>
+      <c r="D31">
+        <v>792.15645908389104</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>2014</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1305.7429718875503</v>
+      </c>
+      <c r="D32">
+        <v>4214.5060240963858</v>
+      </c>
+      <c r="E32">
+        <v>2678.4899598393572</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>2686.7469879518071</v>
+      </c>
+      <c r="D33">
+        <v>4535.7108433734948</v>
+      </c>
+      <c r="E33">
+        <v>2061.8313253012047</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>2014</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>2166.2951807228915</v>
+      </c>
+      <c r="D34">
+        <v>4105.3493975903621</v>
+      </c>
+      <c r="E34">
+        <v>2269.4939759036151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>2014</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>696.78202247191018</v>
+      </c>
+      <c r="D35">
+        <v>1964.2247191011238</v>
+      </c>
+      <c r="E35">
+        <v>856.44943820224728</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>2014</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>684.94082397003751</v>
+      </c>
+      <c r="D36">
+        <v>1927.8651685393261</v>
+      </c>
+      <c r="E36">
+        <v>1264.2247191011236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>671.17153558052439</v>
+      </c>
+      <c r="D37">
+        <v>1894.3071161048688</v>
+      </c>
+      <c r="E37">
+        <v>1128.0898876404494</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>2015</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>2015</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>2686.1686746987953</v>
+      </c>
+      <c r="D39">
+        <v>1986.9397590361443</v>
+      </c>
+      <c r="E39">
+        <v>466.82730923694794</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>2015</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>3083.5662650602412</v>
+      </c>
+      <c r="D40">
+        <v>2146.265060240964</v>
+      </c>
+      <c r="E40">
+        <v>497.34939759036143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>2015</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>3169.5180722891573</v>
+      </c>
+      <c r="D41">
+        <v>1910.439759036145</v>
+      </c>
+      <c r="E41">
+        <v>451.68674698795184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>2016</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>5446.4489795918362</v>
+      </c>
+      <c r="D42">
+        <v>2182.9795918367349</v>
+      </c>
+      <c r="E42">
+        <v>1461.1564625850342</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>2016</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>6036.4625850340144</v>
+      </c>
+      <c r="D43">
+        <v>3420.408163265306</v>
+      </c>
+      <c r="E43">
+        <v>1835.5374149659867</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>2016</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>5673.3061224489802</v>
+      </c>
+      <c r="D44">
+        <v>3043.591836734694</v>
+      </c>
+      <c r="E44">
+        <v>1891.2108843537417</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>2016</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>2017</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>4114.0797546012273</v>
+      </c>
+      <c r="D46">
+        <v>3887.1165644171788</v>
+      </c>
+      <c r="E46">
+        <v>477.66871165644176</v>
+      </c>
+      <c r="F46">
+        <v>776.80981595092032</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>2017</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>4234.4478527607371</v>
+      </c>
+      <c r="D47">
+        <v>3887.1165644171788</v>
+      </c>
+      <c r="E47">
+        <v>444.66257668711654</v>
+      </c>
+      <c r="F47">
+        <v>853.74233128834373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>2017</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>3977.0245398773013</v>
+      </c>
+      <c r="D48">
+        <v>3887.1165644171788</v>
+      </c>
+      <c r="E48">
+        <v>511.28834355828224</v>
+      </c>
+      <c r="F48">
+        <v>702.3312883435583</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>2017</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>1299.591836734694</v>
+      </c>
+      <c r="D49">
+        <v>866.31292517006818</v>
+      </c>
+      <c r="E49">
+        <v>780.27210884353747</v>
+      </c>
+      <c r="F49">
+        <v>300.96598639455777</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>2017</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>1201.6326530612246</v>
+      </c>
+      <c r="D50">
+        <v>1825.8503401360547</v>
+      </c>
+      <c r="E50">
+        <v>675.26530612244892</v>
+      </c>
+      <c r="F50">
+        <v>524.76190476190493</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>2017</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>1442.6666666666667</v>
+      </c>
+      <c r="D51">
+        <v>1355.1020408163265</v>
+      </c>
+      <c r="E51">
+        <v>632.81632653061229</v>
+      </c>
+      <c r="F51">
+        <v>267.30612244897969</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>2018</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>4135.0701402805607</v>
+      </c>
+      <c r="D52">
+        <v>3703.358717434869</v>
+      </c>
+      <c r="E52">
+        <v>298.19639278557116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>2018</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>4409.2184368737471</v>
+      </c>
+      <c r="D53">
+        <v>3163.7675350701402</v>
+      </c>
+      <c r="E53">
+        <v>411.62324649298597</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>2018</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>4995.2104208416831</v>
+      </c>
+      <c r="D54">
+        <v>2879.3587174348695</v>
+      </c>
+      <c r="E54">
+        <v>865.13026052104203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>2018</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>690.18404907975457</v>
+      </c>
+      <c r="D55">
+        <v>1217.6687116564417</v>
+      </c>
+      <c r="E55">
+        <v>245.398773006135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>2018</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>620.85889570552149</v>
+      </c>
+      <c r="D56">
+        <v>1189.1257668711658</v>
+      </c>
+      <c r="E56">
+        <v>245.398773006135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>2018</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>761.96319018404915</v>
+      </c>
+      <c r="D57">
+        <v>1245.5981595092028</v>
+      </c>
+      <c r="E57">
+        <v>245.398773006135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>2019</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>3681.8909090909092</v>
+      </c>
+      <c r="D58">
+        <v>2416.4848484848485</v>
+      </c>
+      <c r="E58">
+        <v>921.21212121212125</v>
+      </c>
+      <c r="F58">
+        <v>277.33333333333331</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>2019</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>3741.4787878787884</v>
+      </c>
+      <c r="D59">
+        <v>3058.424242424242</v>
+      </c>
+      <c r="E59">
+        <v>1336.2424242424242</v>
+      </c>
+      <c r="F59">
+        <v>840.72727272727263</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>2019</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>3711.6848484848488</v>
+      </c>
+      <c r="D60">
+        <v>2737.454545454545</v>
+      </c>
+      <c r="E60">
+        <v>1128.7272727272727</v>
+      </c>
+      <c r="F60">
+        <v>559.030303030303</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>2019</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>1149.0981963927854</v>
+      </c>
+      <c r="D61">
+        <v>742.36472945891774</v>
+      </c>
+      <c r="E61">
+        <v>1226.4529058116232</v>
+      </c>
+      <c r="F61">
+        <v>396.79358717434866</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>2019</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>858.51703406813624</v>
+      </c>
+      <c r="D62">
+        <v>1483.9278557114226</v>
+      </c>
+      <c r="E62">
+        <v>923.0460921843686</v>
+      </c>
+      <c r="F62">
+        <v>312.22444889779558</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>2019</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>825</v>
+      </c>
+      <c r="D63">
+        <v>1418.7374749498995</v>
+      </c>
+      <c r="E63">
+        <v>586.97394789579164</v>
+      </c>
+      <c r="F63">
+        <v>364.72945891783564</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>2020</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>7879.8978461538463</v>
+      </c>
+      <c r="D64">
+        <v>2929.2307692307695</v>
+      </c>
+      <c r="E64">
+        <v>1181.5384615384614</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>2020</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>9119.6451282051312</v>
+      </c>
+      <c r="D65">
+        <v>3532.3076923076924</v>
+      </c>
+      <c r="E65">
+        <v>2038.9743589743591</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <v>2020</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>8499.7714871794888</v>
+      </c>
+      <c r="D66">
+        <v>3230.7692307692309</v>
+      </c>
+      <c r="E66">
+        <v>1610.2564102564104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>2020</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>1418.8450909999999</v>
+      </c>
+      <c r="D67">
+        <v>1181.090909</v>
+      </c>
+      <c r="E67">
+        <v>230.787879</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>2020</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>4831.7352729999993</v>
+      </c>
+      <c r="D68">
+        <v>1838.5454549999999</v>
+      </c>
+      <c r="E68">
+        <v>200.72727300000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <v>2020</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69">
+        <v>3125.2901820000002</v>
+      </c>
+      <c r="D69">
+        <v>1509.818182</v>
+      </c>
+      <c r="E69">
+        <v>215.757576</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70">
+        <v>2021</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>6117.4954954954974</v>
+      </c>
+      <c r="D70">
+        <v>2163.2432432432433</v>
+      </c>
+      <c r="E70">
+        <v>1834.2702702702702</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>2021</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>6317.0270270270266</v>
+      </c>
+      <c r="D71">
+        <v>2220.5405405405404</v>
+      </c>
+      <c r="E71">
+        <v>1785.3153153153153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>2021</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>7243.9639639639636</v>
+      </c>
+      <c r="D72">
+        <v>3035.6756756756758</v>
+      </c>
+      <c r="E72">
+        <v>2296.432432432433</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>2021</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>1227.4871794871794</v>
+      </c>
+      <c r="D73">
+        <v>731.07692307692298</v>
+      </c>
+      <c r="E73">
+        <v>336.41025641025647</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74">
+        <v>2021</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>1662.0307692307692</v>
+      </c>
+      <c r="D74">
+        <v>1011.2820512820513</v>
+      </c>
+      <c r="E74">
+        <v>1122.4615384615383</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
+        <v>2021</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>1452.676923076923</v>
+      </c>
+      <c r="D75">
+        <v>868.30769230769226</v>
+      </c>
+      <c r="E75">
+        <v>702.8717948717948</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <v>2022</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>10477.720430107525</v>
+      </c>
+      <c r="D76">
+        <v>2774.1935483870966</v>
+      </c>
+      <c r="E76">
+        <v>311.61290322580641</v>
+      </c>
+      <c r="F76">
+        <v>193.54838709677418</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <v>2022</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>10260</v>
+      </c>
+      <c r="D77">
+        <v>4236.5591397849457</v>
+      </c>
+      <c r="E77">
+        <v>835.69892473118284</v>
+      </c>
+      <c r="F77">
+        <v>50.806451612903217</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <v>2022</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>11109.032258064517</v>
+      </c>
+      <c r="D78">
+        <v>3343.6559139784945</v>
+      </c>
+      <c r="E78">
+        <v>611.61290322580646</v>
+      </c>
+      <c r="F78">
+        <v>137.63440860215053</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79">
+        <v>2022</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79">
+        <v>1826.7387387387389</v>
+      </c>
+      <c r="D79">
+        <v>3200.9009009009014</v>
+      </c>
+      <c r="E79">
+        <v>113.51351351351352</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80">
+        <v>2022</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80">
+        <v>1729.7297297297296</v>
+      </c>
+      <c r="D80">
+        <v>2492.2522522522522</v>
+      </c>
+      <c r="E80">
+        <v>98.918918918918919</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>2022</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81">
+        <v>2601.5135135135138</v>
+      </c>
+      <c r="D81">
+        <v>3087.9279279279276</v>
+      </c>
+      <c r="E81">
+        <v>571.89189189189187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82AB3A47-C239-47F1-A44D-D2A3CF91BC78}">
+  <dimension ref="A1:H81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>2009</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>1.8</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2009</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1.8</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>2009</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>1.8</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>2009</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>1.8</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>2009</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>3.6</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>2009</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>1.8</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>2010</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>5.4</v>
+      </c>
+      <c r="H8">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>2010</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>3.6</v>
+      </c>
+      <c r="H9">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>2010</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>3.6</v>
+      </c>
+      <c r="H10">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>5.4</v>
+      </c>
+      <c r="H11">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>3.6</v>
+      </c>
+      <c r="H12">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>2010</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>22.222222222222221</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>4.5</v>
+      </c>
+      <c r="G13">
+        <v>3.6</v>
+      </c>
+      <c r="H13">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>2011</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>2011</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>2011</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>1.8</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>2011</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>1.8</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>2011</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1.8</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>2012</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>7.2</v>
+      </c>
+      <c r="H20">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>2012</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>100</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>7.2</v>
+      </c>
+      <c r="H21">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>2012</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>88.888888888888886</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <v>5.4</v>
+      </c>
+      <c r="H22">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>2012</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>5.4</v>
+      </c>
+      <c r="H23">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>5.4</v>
+      </c>
+      <c r="H24">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>5.4</v>
+      </c>
+      <c r="H25">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="G26">
+        <v>5.4</v>
+      </c>
+      <c r="H26">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>2013</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>5.4</v>
+      </c>
+      <c r="H27">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>2013</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>44.444444444444443</v>
+      </c>
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="F28">
+        <v>9</v>
+      </c>
+      <c r="G28">
+        <v>5.4</v>
+      </c>
+      <c r="H28">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>2013</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>5.4</v>
+      </c>
+      <c r="H29">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>2013</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>5.4</v>
+      </c>
+      <c r="H30">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>2013</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>5.4</v>
+      </c>
+      <c r="H31">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>2014</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <v>2.7</v>
+      </c>
+      <c r="H32">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>2.7</v>
+      </c>
+      <c r="H33">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>2014</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>9</v>
+      </c>
+      <c r="G34">
+        <v>2.7</v>
+      </c>
+      <c r="H34">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>2014</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E35">
+        <v>9</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>5.4</v>
+      </c>
+      <c r="H35">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>2014</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>5.4</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>22.222222222222221</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>7</v>
+      </c>
+      <c r="G37">
+        <v>5.4</v>
+      </c>
+      <c r="H37">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <v>2015</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>2015</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>7.5</v>
+      </c>
+      <c r="D39">
+        <v>83.333333333333329</v>
+      </c>
+      <c r="E39">
+        <v>9</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+      <c r="G39">
+        <v>3.6</v>
+      </c>
+      <c r="H39">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>2015</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E40">
+        <v>9</v>
+      </c>
+      <c r="F40">
+        <v>7</v>
+      </c>
+      <c r="G40">
+        <v>3.6</v>
+      </c>
+      <c r="H40">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>2015</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>6.25</v>
+      </c>
+      <c r="D41">
+        <v>69.444444444444443</v>
+      </c>
+      <c r="E41">
+        <v>9</v>
+      </c>
+      <c r="F41">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>4.5</v>
+      </c>
+      <c r="H41">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>2016</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D42">
+        <v>92.222222222222229</v>
+      </c>
+      <c r="E42">
+        <v>9</v>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>1.8</v>
+      </c>
+      <c r="H42">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>2016</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>8.1</v>
+      </c>
+      <c r="D43">
+        <v>90</v>
+      </c>
+      <c r="E43">
+        <v>9</v>
+      </c>
+      <c r="F43">
+        <v>9</v>
+      </c>
+      <c r="G43">
+        <v>1.8</v>
+      </c>
+      <c r="H43">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>2016</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D44">
+        <v>91.1111111111111</v>
+      </c>
+      <c r="E44">
+        <v>8.5</v>
+      </c>
+      <c r="F44">
+        <v>9</v>
+      </c>
+      <c r="G44">
+        <v>2.7</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>2016</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>2017</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>88.888888888888886</v>
+      </c>
+      <c r="E46">
+        <v>9</v>
+      </c>
+      <c r="F46">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>3.6</v>
+      </c>
+      <c r="H46">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>2017</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>88.888888888888886</v>
+      </c>
+      <c r="E47">
+        <v>9</v>
+      </c>
+      <c r="F47">
+        <v>9</v>
+      </c>
+      <c r="G47">
+        <v>3.6</v>
+      </c>
+      <c r="H47">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>2017</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>88.888888888888886</v>
+      </c>
+      <c r="E48">
+        <v>9</v>
+      </c>
+      <c r="F48">
+        <v>9</v>
+      </c>
+      <c r="G48">
+        <v>1.8</v>
+      </c>
+      <c r="H48">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>2017</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49">
+        <v>9</v>
+      </c>
+      <c r="G49">
+        <v>3.6</v>
+      </c>
+      <c r="H49">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>2017</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E50">
+        <v>8.5</v>
+      </c>
+      <c r="F50">
+        <v>7</v>
+      </c>
+      <c r="G50">
+        <v>3.6</v>
+      </c>
+      <c r="H50">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>2017</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E51">
+        <v>8.5</v>
+      </c>
+      <c r="F51">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <v>4.5</v>
+      </c>
+      <c r="H51">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>2018</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>66.666666666666671</v>
+      </c>
+      <c r="E52">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <v>9</v>
+      </c>
+      <c r="G52">
+        <v>3.6</v>
+      </c>
+      <c r="H52">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>2018</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>100</v>
+      </c>
+      <c r="E53">
+        <v>9</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>3.6</v>
+      </c>
+      <c r="H53">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>2018</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>7.5</v>
+      </c>
+      <c r="D54">
+        <v>83.333333333333329</v>
+      </c>
+      <c r="E54">
+        <v>9</v>
+      </c>
+      <c r="F54">
+        <v>6</v>
+      </c>
+      <c r="G54">
+        <v>3.6</v>
+      </c>
+      <c r="H54">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55">
+        <v>2018</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>5.75</v>
+      </c>
+      <c r="G55">
+        <v>3.24</v>
+      </c>
+      <c r="H55">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56">
+        <v>2018</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>44.444444444444443</v>
+      </c>
+      <c r="E56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>5.75</v>
+      </c>
+      <c r="G56">
+        <v>3.6</v>
+      </c>
+      <c r="H56">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>2018</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E57">
+        <v>6</v>
+      </c>
+      <c r="F57">
+        <v>5.75</v>
+      </c>
+      <c r="G57">
+        <v>3.6</v>
+      </c>
+      <c r="H57">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>2019</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>9</v>
+      </c>
+      <c r="D58">
+        <v>100</v>
+      </c>
+      <c r="E58">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>7.5</v>
+      </c>
+      <c r="G58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H58">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59">
+        <v>2019</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>8.6</v>
+      </c>
+      <c r="D59">
+        <v>95.555555555555557</v>
+      </c>
+      <c r="E59">
+        <v>9</v>
+      </c>
+      <c r="F59">
+        <v>7</v>
+      </c>
+      <c r="G59">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <v>2019</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D60">
+        <v>97.777777777777786</v>
+      </c>
+      <c r="E60">
+        <v>9</v>
+      </c>
+      <c r="F60">
+        <v>7</v>
+      </c>
+      <c r="G60">
+        <v>2.7</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61">
+        <v>2019</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>5.5</v>
+      </c>
+      <c r="D61">
+        <v>61.111111111111114</v>
+      </c>
+      <c r="E61">
+        <v>7</v>
+      </c>
+      <c r="F61">
+        <v>9</v>
+      </c>
+      <c r="G61">
+        <v>1.8</v>
+      </c>
+      <c r="H61">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62">
+        <v>2019</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>44.444444444444443</v>
+      </c>
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="F62">
+        <v>8</v>
+      </c>
+      <c r="G62">
+        <v>1.8</v>
+      </c>
+      <c r="H62">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63">
+        <v>2019</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>4.5</v>
+      </c>
+      <c r="D63">
+        <v>50</v>
+      </c>
+      <c r="E63">
+        <v>6</v>
+      </c>
+      <c r="F63">
+        <v>8</v>
+      </c>
+      <c r="G63">
+        <v>1.8</v>
+      </c>
+      <c r="H63">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64">
+        <v>2020</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>9</v>
+      </c>
+      <c r="D64">
+        <v>100</v>
+      </c>
+      <c r="E64">
+        <v>8</v>
+      </c>
+      <c r="F64">
+        <v>7.75</v>
+      </c>
+      <c r="G64">
+        <v>2.7</v>
+      </c>
+      <c r="H64">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65">
+        <v>2020</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>9</v>
+      </c>
+      <c r="D65">
+        <v>100</v>
+      </c>
+      <c r="E65">
+        <v>8.5</v>
+      </c>
+      <c r="F65">
+        <v>7.1</v>
+      </c>
+      <c r="G65">
+        <v>3.6</v>
+      </c>
+      <c r="H65">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66">
+        <v>2020</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+      <c r="D66">
+        <v>100</v>
+      </c>
+      <c r="E66">
+        <v>8.25</v>
+      </c>
+      <c r="F66">
+        <v>7.4249999999999998</v>
+      </c>
+      <c r="G66">
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="H66">
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67">
+        <v>2020</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>8</v>
+      </c>
+      <c r="D67">
+        <v>88.888888888888886</v>
+      </c>
+      <c r="E67">
+        <v>6.25</v>
+      </c>
+      <c r="F67">
+        <v>6.5</v>
+      </c>
+      <c r="G67">
+        <v>2.7</v>
+      </c>
+      <c r="H67">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68">
+        <v>2020</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>9</v>
+      </c>
+      <c r="D68">
+        <v>100</v>
+      </c>
+      <c r="E68">
+        <v>7.5</v>
+      </c>
+      <c r="F68">
+        <v>5.5</v>
+      </c>
+      <c r="G68">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69">
+        <v>2020</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69">
+        <v>8.5</v>
+      </c>
+      <c r="D69">
+        <v>94.444444444444443</v>
+      </c>
+      <c r="E69">
+        <v>6.875</v>
+      </c>
+      <c r="F69">
+        <v>6.5</v>
+      </c>
+      <c r="G69">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70">
+        <v>2021</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>9</v>
+      </c>
+      <c r="D70">
+        <v>100</v>
+      </c>
+      <c r="E70">
+        <v>9</v>
+      </c>
+      <c r="F70">
+        <v>9</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>3.2399999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71">
+        <v>2021</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>8.9</v>
+      </c>
+      <c r="D71">
+        <v>98.888888888888886</v>
+      </c>
+      <c r="E71">
+        <v>9</v>
+      </c>
+      <c r="F71">
+        <v>8</v>
+      </c>
+      <c r="G71">
+        <v>2.5799999999999996</v>
+      </c>
+      <c r="H71">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72">
+        <v>2021</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D72">
+        <v>97.777777777777786</v>
+      </c>
+      <c r="E72">
+        <v>9</v>
+      </c>
+      <c r="F72">
+        <v>8.5</v>
+      </c>
+      <c r="G72">
+        <v>2.8799999999999994</v>
+      </c>
+      <c r="H72">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73">
+        <v>2021</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>4.5</v>
+      </c>
+      <c r="D73">
+        <v>50</v>
+      </c>
+      <c r="E73">
+        <v>6</v>
+      </c>
+      <c r="F73">
+        <v>6.75</v>
+      </c>
+      <c r="G73">
+        <v>1.8</v>
+      </c>
+      <c r="H73">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74">
+        <v>2021</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>7</v>
+      </c>
+      <c r="D74">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <v>6.75</v>
+      </c>
+      <c r="G74">
+        <v>3.6</v>
+      </c>
+      <c r="H74">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75">
+        <v>2021</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E75">
+        <v>7</v>
+      </c>
+      <c r="F75">
+        <v>7</v>
+      </c>
+      <c r="G75">
+        <v>3.6</v>
+      </c>
+      <c r="H75">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76">
+        <v>2022</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>9</v>
+      </c>
+      <c r="D76">
+        <v>100</v>
+      </c>
+      <c r="E76">
+        <v>9</v>
+      </c>
+      <c r="F76">
+        <v>7.2666666666666666</v>
+      </c>
+      <c r="G76">
+        <v>2.46</v>
+      </c>
+      <c r="H76">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77">
+        <v>2022</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>100</v>
+      </c>
+      <c r="E77">
+        <v>9</v>
+      </c>
+      <c r="F77">
+        <v>6.5333333333333341</v>
+      </c>
+      <c r="G77">
+        <v>2.4</v>
+      </c>
+      <c r="H77">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78">
+        <v>2022</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>9</v>
+      </c>
+      <c r="D78">
+        <v>100</v>
+      </c>
+      <c r="E78">
+        <v>9</v>
+      </c>
+      <c r="F78">
+        <v>7</v>
+      </c>
+      <c r="G78">
+        <v>1.8</v>
+      </c>
+      <c r="H78">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79">
+        <v>2022</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79">
+        <v>7</v>
+      </c>
+      <c r="D79">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E79">
+        <v>6.5</v>
+      </c>
+      <c r="F79">
+        <v>5.166666666666667</v>
+      </c>
+      <c r="G79">
+        <v>2.4299999999999997</v>
+      </c>
+      <c r="H79">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80">
+        <v>2022</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80">
+        <v>7</v>
+      </c>
+      <c r="D80">
+        <v>77.777777777777771</v>
+      </c>
+      <c r="E80">
+        <v>6.8</v>
+      </c>
+      <c r="F80">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="G80">
+        <v>2.79</v>
+      </c>
+      <c r="H80">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81">
+        <v>2022</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="D81">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E81">
+        <v>7</v>
+      </c>
+      <c r="F81">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="G81">
+        <v>2.25</v>
+      </c>
+      <c r="H81">
+        <v>5.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52F5301-2E06-4909-9823-DA2985429D06}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2009</v>
+      </c>
+      <c r="B2">
+        <v>8.57</v>
+      </c>
+      <c r="C2">
+        <v>25.1</v>
+      </c>
+      <c r="D2">
+        <v>68.2</v>
+      </c>
+      <c r="E2">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2009</v>
+      </c>
+      <c r="B3">
+        <v>8.59</v>
+      </c>
+      <c r="C3">
+        <v>24.8</v>
+      </c>
+      <c r="D3">
+        <v>70.3</v>
+      </c>
+      <c r="E3">
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2009</v>
+      </c>
+      <c r="B4">
+        <v>8.58</v>
+      </c>
+      <c r="C4">
+        <v>24.950000000000003</v>
+      </c>
+      <c r="D4">
+        <v>69.25</v>
+      </c>
+      <c r="E4">
+        <v>27.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>2010</v>
+      </c>
+      <c r="B5">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="C5">
+        <v>21.5</v>
+      </c>
+      <c r="D5">
+        <v>79.5</v>
+      </c>
+      <c r="E5">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>2010</v>
+      </c>
+      <c r="B6">
+        <v>9.35</v>
+      </c>
+      <c r="C6">
+        <v>21.3</v>
+      </c>
+      <c r="D6">
+        <v>80.5</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>2010</v>
+      </c>
+      <c r="B7">
+        <v>9.3999999999999986</v>
+      </c>
+      <c r="C7">
+        <v>21.4</v>
+      </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2021</v>
+      </c>
+      <c r="B8">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C8">
+        <v>30.4</v>
+      </c>
+      <c r="D8">
+        <v>67.5</v>
+      </c>
+      <c r="E8">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2021</v>
+      </c>
+      <c r="B9">
+        <v>8.65</v>
+      </c>
+      <c r="C9">
+        <v>27.8</v>
+      </c>
+      <c r="D9">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="E9">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>2021</v>
+      </c>
+      <c r="B10">
+        <v>8.4250000000000007</v>
+      </c>
+      <c r="C10">
+        <v>29.1</v>
+      </c>
+      <c r="D10">
+        <v>71.55</v>
+      </c>
+      <c r="E10">
+        <v>26.700000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2022</v>
+      </c>
+      <c r="B11">
+        <v>10.3</v>
+      </c>
+      <c r="C11">
+        <v>27.1</v>
+      </c>
+      <c r="D11">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="E11">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>2022</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>26.4</v>
+      </c>
+      <c r="D12">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="E12">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2022</v>
+      </c>
+      <c r="B13">
+        <v>10.65</v>
+      </c>
+      <c r="C13">
+        <v>26.75</v>
+      </c>
+      <c r="D13">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="E13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>